<commit_message>
feat: Update plot generation and data handling in PlotService
- Added new plots for MARS Multi Illumination analysis including Boxplots, Grouped Bar charts, and QQ plots.
- Introduced a comparison report PDF summarizing the results.
- Modified file naming conventions for input data to reflect changes in the data structure.
- Enhanced the grouped bar plotting function to display means and standard deviations for both 'WITH' and 'INLIER' datasets.
- Updated logging to provide clearer insights into the data loading process.
- Added new binary files for generated plots and updated existing ones.
</commit_message>
<xml_diff>
--- a/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="134">
   <si>
     <t>Calculated on all distances (incl. Outliers)</t>
   </si>
@@ -258,6 +258,9 @@
     <t>data\Multi-illumination\Job_0378_8400-110\1-1</t>
   </si>
   <si>
+    <t>AI_cloud vs. cloud</t>
+  </si>
+  <si>
     <t>std</t>
   </si>
   <si>
@@ -339,7 +342,88 @@
     <t>data\Multi-illumination\Job_0378_8400-110\1-7\python_Job_0378_8400-110-rad-1-7-AI_cloud_m3c2_params.txt</t>
   </si>
   <si>
-    <t>AI_cloud vs. cloud</t>
+    <t>2025-08-27 15:47:40</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-1-5-AI_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-1-5-AI_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:52:08</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-2-5-AI_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-2-5-AI_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-27 15:56:34</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-1-5_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-5_2-5\python_Job_0378_8400-110-rad-1-5_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-27 16:37:38</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_1-3_AI</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_1-3_AI\python_Job_0378_8400-110-rad-1-3-AI_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_1-3_AI\python_Job_0378_8400-110-rad-1-3-AI_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-27 16:40:33</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_2-3</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_2-3\python_Job_0378_8400-110-rad-1-3_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\1-3_2-3\python_Job_0378_8400-110-rad-1-3_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>2025-08-27 16:43:47</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\2-3_2-3_AI</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\2-3_2-3_AI\python_Job_0378_8400-110-rad-2-3_cloud_moved_m3c2_distances.txt</t>
+  </si>
+  <si>
+    <t>data\Multi-illumination\Job_0378_8400-110\1-3_2-3\2-3_2-3_AI\python_Job_0378_8400-110-rad-2-3_cloud_moved_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>1-3_1-3_AI</t>
+  </si>
+  <si>
+    <t>1-3_2-3</t>
+  </si>
+  <si>
+    <t>2-3_2-3_AI</t>
+  </si>
+  <si>
+    <t>1-5_1-5_AI</t>
+  </si>
+  <si>
+    <t>2-5_2-5_AI</t>
+  </si>
+  <si>
+    <t>1-5_2-5</t>
   </si>
 </sst>
 </file>
@@ -419,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -494,6 +578,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -501,9 +594,6 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -539,11 +629,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -551,15 +651,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,333 +956,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM9"/>
+  <dimension ref="A1:BM15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="17" style="13" customWidth="1"/>
-    <col min="5" max="6" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="31" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.42578125" style="13" customWidth="1"/>
-    <col min="33" max="33" width="12.28515625" style="13" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" style="13" customWidth="1"/>
-    <col min="36" max="39" width="9.85546875" style="13" customWidth="1"/>
-    <col min="41" max="54" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.85546875" style="13" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="17" style="13" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.7109375" style="13" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="10.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="46.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="44.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="66" max="72" width="9.140625" style="13" customWidth="1"/>
-    <col min="73" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="6" width="7.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="31" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.42578125" style="12" customWidth="1"/>
+    <col min="33" max="33" width="12.28515625" style="12" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" style="12" customWidth="1"/>
+    <col min="36" max="39" width="9.85546875" style="12" customWidth="1"/>
+    <col min="41" max="54" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.85546875" style="12" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.7109375" style="12" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="125.42578125" style="12" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="44.5703125" style="12" hidden="1" customWidth="1"/>
+    <col min="66" max="73" width="9.140625" style="12" customWidth="1"/>
+    <col min="74" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="19" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="15" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="20" t="s">
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="21" t="s">
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="22" t="s">
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="19" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="15" t="s">
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="18"/>
+      <c r="BA1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="16"/>
-      <c r="BE1" s="16"/>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="18"/>
     </row>
-    <row r="2" spans="1:65" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:65" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="23" t="s">
+      <c r="T2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AE2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="AF2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" s="14" t="s">
+      <c r="AG2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AH2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AI2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="AK2" s="11" t="s">
+      <c r="AK2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AL2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AM2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AN2" s="12" t="s">
+      <c r="AN2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AO2" s="12" t="s">
+      <c r="AO2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AP2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AR2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AS2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AU2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AV2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AW2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AX2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AY2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BA2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BB2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BC2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BD2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BE2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BF2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BG2" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BH2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BI2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BJ2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BK2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BL2" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BM2" s="14" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1203,7 +1295,7 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>1848754</v>
@@ -1296,7 +1388,7 @@
         <v>2.8987225010835092E-3</v>
       </c>
       <c r="AH3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI3">
         <v>1828425</v>
@@ -1386,21 +1478,21 @@
         <v>0.70709521600129976</v>
       </c>
       <c r="BL3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="BM3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>105</v>
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
       </c>
       <c r="D4">
         <v>1878902</v>
@@ -1493,7 +1585,7 @@
         <v>2.3642819230001448E-3</v>
       </c>
       <c r="AH4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI4">
         <v>1839658</v>
@@ -1583,21 +1675,21 @@
         <v>2.633819827986851</v>
       </c>
       <c r="BL4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="BM4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>105</v>
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
       </c>
       <c r="D5">
         <v>1900069</v>
@@ -1690,7 +1782,7 @@
         <v>2.7529500676348379E-3</v>
       </c>
       <c r="AH5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI5">
         <v>1864352</v>
@@ -1780,21 +1872,21 @@
         <v>1.9867408025238671</v>
       </c>
       <c r="BL5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="BM5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
       </c>
       <c r="D6">
         <v>1801484</v>
@@ -1887,7 +1979,7 @@
         <v>2.2612950850070261E-3</v>
       </c>
       <c r="AH6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI6">
         <v>1763317</v>
@@ -1977,21 +2069,21 @@
         <v>2.5684437604908958</v>
       </c>
       <c r="BL6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="BM6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
       </c>
       <c r="D7">
         <v>1838147</v>
@@ -2084,7 +2176,7 @@
         <v>2.592776601724162E-3</v>
       </c>
       <c r="AH7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI7">
         <v>1815047</v>
@@ -2174,21 +2266,21 @@
         <v>1.6998174583202921</v>
       </c>
       <c r="BL7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BM7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
       </c>
       <c r="D8">
         <v>1843820</v>
@@ -2281,7 +2373,7 @@
         <v>2.393666029402013E-3</v>
       </c>
       <c r="AH8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI8">
         <v>1821523</v>
@@ -2371,207 +2463,1389 @@
         <v>1.244933915807767</v>
       </c>
       <c r="BL8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BM8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:65" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1796164</v>
+      </c>
+      <c r="E9" s="15">
+        <v>2E-3</v>
+      </c>
+      <c r="F9" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="15">
+        <v>4545</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2.530392547673821E-3</v>
+      </c>
+      <c r="I9" s="15">
+        <v>0.99746960745232616</v>
+      </c>
+      <c r="J9" s="15">
+        <v>1791619</v>
+      </c>
+      <c r="K9" s="15">
+        <v>-443.82193000000001</v>
+      </c>
+      <c r="L9" s="15">
+        <v>1.2996335951539999</v>
+      </c>
+      <c r="M9" s="15">
+        <v>1765379</v>
+      </c>
+      <c r="N9" s="15">
+        <v>-411.92550499999999</v>
+      </c>
+      <c r="O9" s="15">
+        <v>1.071713381031</v>
+      </c>
+      <c r="P9" s="15">
+        <v>-4.2890000000000003E-3</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>3.9290000000000002E-3</v>
+      </c>
+      <c r="R9" s="15">
+        <v>-2.4772115611633948E-4</v>
+      </c>
+      <c r="S9" s="15">
+        <v>-2.3800000000000001E-4</v>
+      </c>
+      <c r="T9" s="15">
+        <v>8.5170193684826201E-4</v>
+      </c>
+      <c r="U9" s="15">
+        <v>8.1488061582262784E-4</v>
+      </c>
+      <c r="V9" s="15">
+        <v>6.2145386491212695E-4</v>
+      </c>
+      <c r="W9" s="15">
+        <v>5.9007480000000006E-4</v>
+      </c>
+      <c r="X9" s="15">
+        <v>-2.6919999999999999E-3</v>
+      </c>
+      <c r="Y9" s="15">
+        <v>2.196E-3</v>
+      </c>
+      <c r="Z9" s="15">
+        <v>-2.3333545091450619E-4</v>
+      </c>
+      <c r="AA9" s="15">
+        <v>-2.3499999999999999E-4</v>
+      </c>
+      <c r="AB9" s="15">
+        <v>7.7914869664949646E-4</v>
+      </c>
+      <c r="AC9" s="15">
+        <v>7.4338903599470256E-4</v>
+      </c>
+      <c r="AD9" s="15">
+        <v>5.8731266373962749E-4</v>
+      </c>
+      <c r="AE9" s="15">
+        <v>5.7673139999999995E-4</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>3</v>
+      </c>
+      <c r="AG9" s="15">
+        <v>2.4446418474678841E-3</v>
+      </c>
+      <c r="AH9" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI9" s="15">
+        <v>1765379</v>
+      </c>
+      <c r="AJ9" s="15">
+        <v>584283</v>
+      </c>
+      <c r="AK9" s="15">
+        <v>1180017</v>
+      </c>
+      <c r="AL9" s="15">
+        <v>8550</v>
+      </c>
+      <c r="AM9" s="15">
+        <v>17690</v>
+      </c>
+      <c r="AN9" s="15">
+        <v>26240</v>
+      </c>
+      <c r="AO9" s="15">
+        <v>-1.2155649771341461E-3</v>
+      </c>
+      <c r="AP9" s="15">
+        <v>2.6848436744615631E-3</v>
+      </c>
+      <c r="AQ9" s="15">
+        <v>-1.6299999999999999E-3</v>
+      </c>
+      <c r="AR9" s="15">
+        <v>-6.3500000000000004E-4</v>
+      </c>
+      <c r="AS9" s="15">
+        <v>1.6100000000000001E-4</v>
+      </c>
+      <c r="AT9" s="15">
+        <v>1.101E-3</v>
+      </c>
+      <c r="AU9" s="15">
+        <v>7.9600000000000005E-4</v>
+      </c>
+      <c r="AV9" s="15">
+        <v>-1.518E-3</v>
+      </c>
+      <c r="AW9" s="15">
+        <v>-6.2E-4</v>
+      </c>
+      <c r="AX9" s="15">
+        <v>1.5899999999999999E-4</v>
+      </c>
+      <c r="AY9" s="15">
+        <v>1.0560000000000001E-3</v>
+      </c>
+      <c r="AZ9" s="15">
+        <v>7.7899999999999996E-4</v>
+      </c>
+      <c r="BA9" s="15">
+        <v>-2.4772115611633948E-4</v>
+      </c>
+      <c r="BB9" s="15">
+        <v>8.1488061582262784E-4</v>
+      </c>
+      <c r="BC9" s="15">
+        <v>578540.15135124186</v>
+      </c>
+      <c r="BD9" s="15">
+        <v>5.2652448874361362</v>
+      </c>
+      <c r="BE9" s="15">
+        <v>4.3633475494600157E-3</v>
+      </c>
+      <c r="BF9" s="15">
+        <v>-4.2896485267772157E-3</v>
+      </c>
+      <c r="BG9" s="15">
+        <v>-9.7404824018398374E-5</v>
+      </c>
+      <c r="BH9" s="15">
+        <v>-0.28937373573272951</v>
+      </c>
+      <c r="BI9" s="15">
+        <v>1560315349.7288761</v>
+      </c>
+      <c r="BJ9" s="15">
+        <v>-0.17371904743128719</v>
+      </c>
+      <c r="BK9" s="15">
+        <v>2.0872163460411568</v>
+      </c>
+      <c r="BL9" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="BM9" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D9">
-        <v>1796164</v>
-      </c>
-      <c r="E9">
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10">
+        <v>1838147</v>
+      </c>
+      <c r="E10">
         <v>2E-3</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G9">
-        <v>4545</v>
-      </c>
-      <c r="H9">
-        <v>2.530392547673821E-3</v>
-      </c>
-      <c r="I9">
-        <v>0.99746960745232616</v>
-      </c>
-      <c r="J9">
-        <v>1791619</v>
-      </c>
-      <c r="K9">
-        <v>-443.82193000000001</v>
-      </c>
-      <c r="L9">
-        <v>1.2996335951539999</v>
-      </c>
-      <c r="M9">
-        <v>1765379</v>
-      </c>
-      <c r="N9">
-        <v>-411.92550499999999</v>
-      </c>
-      <c r="O9">
-        <v>1.071713381031</v>
-      </c>
-      <c r="P9">
-        <v>-4.2890000000000003E-3</v>
-      </c>
-      <c r="Q9">
-        <v>3.9290000000000002E-3</v>
-      </c>
-      <c r="R9">
-        <v>-2.4772115611633948E-4</v>
-      </c>
-      <c r="S9">
-        <v>-2.3800000000000001E-4</v>
-      </c>
-      <c r="T9">
-        <v>8.5170193684826201E-4</v>
-      </c>
-      <c r="U9">
-        <v>8.1488061582262784E-4</v>
-      </c>
-      <c r="V9">
-        <v>6.2145386491212695E-4</v>
-      </c>
-      <c r="W9">
-        <v>5.9007480000000006E-4</v>
-      </c>
-      <c r="X9">
-        <v>-2.6919999999999999E-3</v>
-      </c>
-      <c r="Y9">
-        <v>2.196E-3</v>
-      </c>
-      <c r="Z9">
-        <v>-2.3333545091450619E-4</v>
-      </c>
-      <c r="AA9">
-        <v>-2.3499999999999999E-4</v>
-      </c>
-      <c r="AB9">
-        <v>7.7914869664949646E-4</v>
-      </c>
-      <c r="AC9">
-        <v>7.4338903599470256E-4</v>
-      </c>
-      <c r="AD9">
-        <v>5.8731266373962749E-4</v>
-      </c>
-      <c r="AE9">
-        <v>5.7673139999999995E-4</v>
-      </c>
-      <c r="AF9">
+      <c r="G10">
+        <v>2713</v>
+      </c>
+      <c r="H10">
+        <v>1.475942892489012E-3</v>
+      </c>
+      <c r="I10">
+        <v>0.99852405710751102</v>
+      </c>
+      <c r="J10">
+        <v>1835434</v>
+      </c>
+      <c r="K10">
+        <v>-707.39812299999994</v>
+      </c>
+      <c r="L10">
+        <v>1.643617490499</v>
+      </c>
+      <c r="M10">
+        <v>1815039</v>
+      </c>
+      <c r="N10">
+        <v>-709.53198300000008</v>
+      </c>
+      <c r="O10">
+        <v>1.464372709929</v>
+      </c>
+      <c r="P10">
+        <v>-4.3600000000000002E-3</v>
+      </c>
+      <c r="Q10">
+        <v>3.9490000000000003E-3</v>
+      </c>
+      <c r="R10">
+        <v>-3.8541190966278271E-4</v>
+      </c>
+      <c r="S10">
+        <v>-3.3799999999999998E-4</v>
+      </c>
+      <c r="T10">
+        <v>9.4630468641177413E-4</v>
+      </c>
+      <c r="U10">
+        <v>8.6426281848461654E-4</v>
+      </c>
+      <c r="V10">
+        <v>6.9650989084870383E-4</v>
+      </c>
+      <c r="W10">
+        <v>6.0786599999999998E-4</v>
+      </c>
+      <c r="X10">
+        <v>-2.9780000000000002E-3</v>
+      </c>
+      <c r="Y10">
+        <v>2.2070000000000002E-3</v>
+      </c>
+      <c r="Z10">
+        <v>-3.9091831249907032E-4</v>
+      </c>
+      <c r="AA10">
+        <v>-3.39E-4</v>
+      </c>
+      <c r="AB10">
+        <v>8.9822023128054108E-4</v>
+      </c>
+      <c r="AC10">
+        <v>8.0869181820675544E-4</v>
+      </c>
+      <c r="AD10">
+        <v>6.7138149152717939E-4</v>
+      </c>
+      <c r="AE10">
+        <v>5.9897039999999991E-4</v>
+      </c>
+      <c r="AF10">
         <v>3</v>
       </c>
-      <c r="AG9">
-        <v>2.4446418474678841E-3</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>78</v>
-      </c>
-      <c r="AI9">
-        <v>1765379</v>
-      </c>
-      <c r="AJ9">
-        <v>584283</v>
-      </c>
-      <c r="AK9">
-        <v>1180017</v>
-      </c>
-      <c r="AL9">
-        <v>8550</v>
-      </c>
-      <c r="AM9">
-        <v>17690</v>
-      </c>
-      <c r="AN9">
-        <v>26240</v>
-      </c>
-      <c r="AO9">
-        <v>-1.2155649771341461E-3</v>
-      </c>
-      <c r="AP9">
-        <v>2.6848436744615631E-3</v>
-      </c>
-      <c r="AQ9">
-        <v>-1.6299999999999999E-3</v>
-      </c>
-      <c r="AR9">
-        <v>-6.3500000000000004E-4</v>
-      </c>
-      <c r="AS9">
+      <c r="AG10">
+        <v>2.5927884554538491E-3</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI10">
+        <v>1815039</v>
+      </c>
+      <c r="AJ10">
+        <v>495610</v>
+      </c>
+      <c r="AK10">
+        <v>1318523</v>
+      </c>
+      <c r="AL10">
+        <v>11567</v>
+      </c>
+      <c r="AM10">
+        <v>8828</v>
+      </c>
+      <c r="AN10">
+        <v>20395</v>
+      </c>
+      <c r="AO10">
+        <v>1.046266241725913E-4</v>
+      </c>
+      <c r="AP10">
+        <v>2.962721081208567E-3</v>
+      </c>
+      <c r="AQ10">
+        <v>-2.0140000000000002E-3</v>
+      </c>
+      <c r="AR10">
+        <v>-7.7200000000000001E-4</v>
+      </c>
+      <c r="AS10">
+        <v>5.3000000000000001E-5</v>
+      </c>
+      <c r="AT10">
+        <v>9.5299999999999996E-4</v>
+      </c>
+      <c r="AU10">
+        <v>8.25E-4</v>
+      </c>
+      <c r="AV10">
+        <v>-1.9610000000000001E-3</v>
+      </c>
+      <c r="AW10">
+        <v>-7.67E-4</v>
+      </c>
+      <c r="AX10">
+        <v>4.6E-5</v>
+      </c>
+      <c r="AY10">
+        <v>8.9099999999999997E-4</v>
+      </c>
+      <c r="AZ10">
+        <v>8.1300000000000003E-4</v>
+      </c>
+      <c r="BA10">
+        <v>-3.8541190966278271E-4</v>
+      </c>
+      <c r="BB10">
+        <v>8.6426281848461654E-4</v>
+      </c>
+      <c r="BC10">
+        <v>393846.34978408553</v>
+      </c>
+      <c r="BD10">
+        <v>4.9305939725702448</v>
+      </c>
+      <c r="BE10">
+        <v>4.3101056020565234E-3</v>
+      </c>
+      <c r="BF10">
+        <v>-4.36032921407242E-3</v>
+      </c>
+      <c r="BG10">
+        <v>-2.4388194603458879E-4</v>
+      </c>
+      <c r="BH10">
+        <v>-0.24436362494983771</v>
+      </c>
+      <c r="BI10">
+        <v>34328485.413518503</v>
+      </c>
+      <c r="BJ10">
+        <v>-0.1597823831466095</v>
+      </c>
+      <c r="BK10">
+        <v>1.6995150221965249</v>
+      </c>
+      <c r="BL10" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11">
+        <v>1836691</v>
+      </c>
+      <c r="E11">
+        <v>2E-3</v>
+      </c>
+      <c r="F11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G11">
+        <v>1825</v>
+      </c>
+      <c r="H11">
+        <v>9.9363474857774121E-4</v>
+      </c>
+      <c r="I11">
+        <v>0.99900636525142228</v>
+      </c>
+      <c r="J11">
+        <v>1834866</v>
+      </c>
+      <c r="K11">
+        <v>-742.21208899999999</v>
+      </c>
+      <c r="L11">
+        <v>1.4993374988570001</v>
+      </c>
+      <c r="M11">
+        <v>1815598</v>
+      </c>
+      <c r="N11">
+        <v>-705.56806200000005</v>
+      </c>
+      <c r="O11">
+        <v>1.327135725142</v>
+      </c>
+      <c r="P11">
+        <v>-4.2110000000000003E-3</v>
+      </c>
+      <c r="Q11">
+        <v>4.0889999999999998E-3</v>
+      </c>
+      <c r="R11">
+        <v>-4.045047916305605E-4</v>
+      </c>
+      <c r="S11">
+        <v>-3.0699999999999998E-4</v>
+      </c>
+      <c r="T11">
+        <v>9.0395648518970789E-4</v>
+      </c>
+      <c r="U11">
+        <v>8.0840163326433684E-4</v>
+      </c>
+      <c r="V11">
+        <v>6.5726197934890061E-4</v>
+      </c>
+      <c r="W11">
+        <v>6.1231379999999991E-4</v>
+      </c>
+      <c r="X11">
+        <v>-2.8289999999999999E-3</v>
+      </c>
+      <c r="Y11">
+        <v>2.0200000000000001E-3</v>
+      </c>
+      <c r="Z11">
+        <v>-3.8861469444227188E-4</v>
+      </c>
+      <c r="AA11">
+        <v>-3.0299999999999999E-4</v>
+      </c>
+      <c r="AB11">
+        <v>8.5496398809868353E-4</v>
+      </c>
+      <c r="AC11">
+        <v>7.6153925716875915E-4</v>
+      </c>
+      <c r="AD11">
+        <v>6.3275608477206962E-4</v>
+      </c>
+      <c r="AE11">
+        <v>6.0341819999999995E-4</v>
+      </c>
+      <c r="AF11">
+        <v>3</v>
+      </c>
+      <c r="AG11">
+        <v>2.4252048997930099E-3</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI11">
+        <v>1815598</v>
+      </c>
+      <c r="AJ11">
+        <v>519784</v>
+      </c>
+      <c r="AK11">
+        <v>1294647</v>
+      </c>
+      <c r="AL11">
+        <v>4107</v>
+      </c>
+      <c r="AM11">
+        <v>15161</v>
+      </c>
+      <c r="AN11">
+        <v>19268</v>
+      </c>
+      <c r="AO11">
+        <v>-1.9018075046709571E-3</v>
+      </c>
+      <c r="AP11">
+        <v>2.3065814637335609E-3</v>
+      </c>
+      <c r="AQ11">
+        <v>-1.9940000000000001E-3</v>
+      </c>
+      <c r="AR11">
+        <v>-7.8200000000000003E-4</v>
+      </c>
+      <c r="AS11">
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="AT11">
+        <v>7.8200000000000003E-4</v>
+      </c>
+      <c r="AU11">
+        <v>8.43E-4</v>
+      </c>
+      <c r="AV11">
+        <v>-1.8929999999999999E-3</v>
+      </c>
+      <c r="AW11">
+        <v>-7.67E-4</v>
+      </c>
+      <c r="AX11">
+        <v>6.0999999999999999E-5</v>
+      </c>
+      <c r="AY11">
+        <v>7.67E-4</v>
+      </c>
+      <c r="AZ11">
+        <v>8.2799999999999996E-4</v>
+      </c>
+      <c r="BA11">
+        <v>-4.045047916305605E-4</v>
+      </c>
+      <c r="BB11">
+        <v>8.0840163326433684E-4</v>
+      </c>
+      <c r="BC11">
+        <v>343158.95979839168</v>
+      </c>
+      <c r="BD11">
+        <v>5.8664235131932916</v>
+      </c>
+      <c r="BE11">
+        <v>4.5046560421914518E-3</v>
+      </c>
+      <c r="BF11">
+        <v>-4.5916351408282719E-3</v>
+      </c>
+      <c r="BG11">
+        <v>-2.282216224772085E-4</v>
+      </c>
+      <c r="BH11">
+        <v>-0.35932232003876979</v>
+      </c>
+      <c r="BI11">
+        <v>1728009635829.803</v>
+      </c>
+      <c r="BJ11">
+        <v>-0.54806856144724914</v>
+      </c>
+      <c r="BK11">
+        <v>1.3917515097410511</v>
+      </c>
+      <c r="BL11" t="s">
+        <v>111</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12">
+        <v>1836691</v>
+      </c>
+      <c r="E12">
+        <v>2E-3</v>
+      </c>
+      <c r="F12">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G12">
+        <v>51076</v>
+      </c>
+      <c r="H12">
+        <v>2.7808705982661209E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.97219129401733884</v>
+      </c>
+      <c r="J12">
+        <v>1785615</v>
+      </c>
+      <c r="K12">
+        <v>-28.935051999999999</v>
+      </c>
+      <c r="L12">
+        <v>0.11496055780800001</v>
+      </c>
+      <c r="M12">
+        <v>1768260</v>
+      </c>
+      <c r="N12">
+        <v>-30.000653</v>
+      </c>
+      <c r="O12">
+        <v>9.2757716744999996E-2</v>
+      </c>
+      <c r="P12">
+        <v>-4.0099999999999997E-3</v>
+      </c>
+      <c r="Q12">
+        <v>4.5319999999999996E-3</v>
+      </c>
+      <c r="R12">
+        <v>-1.6204530091873109E-5</v>
+      </c>
+      <c r="S12">
+        <v>-1.1E-5</v>
+      </c>
+      <c r="T12">
+        <v>2.5373508228747999E-4</v>
+      </c>
+      <c r="U12">
+        <v>2.5321711077242761E-4</v>
+      </c>
+      <c r="V12">
+        <v>1.8778190819409559E-4</v>
+      </c>
+      <c r="W12">
+        <v>2.2090740000000001E-4</v>
+      </c>
+      <c r="X12">
+        <v>-7.7499999999999997E-4</v>
+      </c>
+      <c r="Y12">
+        <v>7.4299999999999995E-4</v>
+      </c>
+      <c r="Z12">
+        <v>-1.696620010631921E-5</v>
+      </c>
+      <c r="AA12">
+        <v>-1.1E-5</v>
+      </c>
+      <c r="AB12">
+        <v>2.2903505766893031E-4</v>
+      </c>
+      <c r="AC12">
+        <v>2.2840579172902451E-4</v>
+      </c>
+      <c r="AD12">
+        <v>1.7952738567857671E-4</v>
+      </c>
+      <c r="AE12">
+        <v>2.1942479999999999E-4</v>
+      </c>
+      <c r="AF12">
+        <v>3</v>
+      </c>
+      <c r="AG12">
+        <v>7.5965133231728271E-4</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI12">
+        <v>1768260</v>
+      </c>
+      <c r="AJ12">
+        <v>846391</v>
+      </c>
+      <c r="AK12">
+        <v>918559</v>
+      </c>
+      <c r="AL12">
+        <v>9115</v>
+      </c>
+      <c r="AM12">
+        <v>8240</v>
+      </c>
+      <c r="AN12">
+        <v>17355</v>
+      </c>
+      <c r="AO12">
+        <v>6.1400230481129355E-5</v>
+      </c>
+      <c r="AP12">
+        <v>1.1294086870939949E-3</v>
+      </c>
+      <c r="AQ12">
+        <v>-4.0499999999999998E-4</v>
+      </c>
+      <c r="AR12">
+        <v>-1.6799999999999999E-4</v>
+      </c>
+      <c r="AS12">
+        <v>1.3100000000000001E-4</v>
+      </c>
+      <c r="AT12">
+        <v>3.6499999999999998E-4</v>
+      </c>
+      <c r="AU12">
+        <v>2.99E-4</v>
+      </c>
+      <c r="AV12">
+        <v>-3.9500000000000001E-4</v>
+      </c>
+      <c r="AW12">
+        <v>-1.6699999999999999E-4</v>
+      </c>
+      <c r="AX12">
+        <v>1.2899999999999999E-4</v>
+      </c>
+      <c r="AY12">
+        <v>3.5300000000000002E-4</v>
+      </c>
+      <c r="AZ12">
+        <v>2.9599999999999998E-4</v>
+      </c>
+      <c r="BA12">
+        <v>-1.6204530091873109E-5</v>
+      </c>
+      <c r="BB12">
+        <v>2.5321711077242761E-4</v>
+      </c>
+      <c r="BC12">
+        <v>22059671856180</v>
+      </c>
+      <c r="BD12">
+        <v>1.0529685505430511</v>
+      </c>
+      <c r="BE12">
+        <v>1.227482360863936E-2</v>
+      </c>
+      <c r="BF12">
+        <v>-3.341000035855021E-3</v>
+      </c>
+      <c r="BG12">
+        <v>-2.6233172121310172E-3</v>
+      </c>
+      <c r="BH12">
+        <v>1.851205647654703</v>
+      </c>
+      <c r="BI12">
+        <v>33036533.891676862</v>
+      </c>
+      <c r="BJ12">
+        <v>0.1863157457628726</v>
+      </c>
+      <c r="BK12">
+        <v>10.93220370089232</v>
+      </c>
+      <c r="BL12" t="s">
+        <v>114</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13">
+        <v>1900069</v>
+      </c>
+      <c r="E13">
+        <v>2E-3</v>
+      </c>
+      <c r="F13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G13">
+        <v>5914</v>
+      </c>
+      <c r="H13">
+        <v>3.112518545379141E-3</v>
+      </c>
+      <c r="I13">
+        <v>0.99688748145462081</v>
+      </c>
+      <c r="J13">
+        <v>1894155</v>
+      </c>
+      <c r="K13">
+        <v>-832.78334999999993</v>
+      </c>
+      <c r="L13">
+        <v>1.961207886892</v>
+      </c>
+      <c r="M13">
+        <v>1864341</v>
+      </c>
+      <c r="N13">
+        <v>-848.03458999999998</v>
+      </c>
+      <c r="O13">
+        <v>1.6842043167859999</v>
+      </c>
+      <c r="P13">
+        <v>-4.7359999999999998E-3</v>
+      </c>
+      <c r="Q13">
+        <v>4.2220000000000001E-3</v>
+      </c>
+      <c r="R13">
+        <v>-4.3965955795592231E-4</v>
+      </c>
+      <c r="S13">
+        <v>-4.35E-4</v>
+      </c>
+      <c r="T13">
+        <v>1.0175460158415449E-3</v>
+      </c>
+      <c r="U13">
+        <v>9.1765972312889794E-4</v>
+      </c>
+      <c r="V13">
+        <v>7.7122022748930266E-4</v>
+      </c>
+      <c r="W13">
+        <v>6.5382659999999992E-4</v>
+      </c>
+      <c r="X13">
+        <v>-3.192E-3</v>
+      </c>
+      <c r="Y13">
+        <v>2.313E-3</v>
+      </c>
+      <c r="Z13">
+        <v>-4.5487096512923327E-4</v>
+      </c>
+      <c r="AA13">
+        <v>-4.3800000000000002E-4</v>
+      </c>
+      <c r="AB13">
+        <v>9.5046190062665202E-4</v>
+      </c>
+      <c r="AC13">
+        <v>8.3454791931034588E-4</v>
+      </c>
+      <c r="AD13">
+        <v>7.3544801407038731E-4</v>
+      </c>
+      <c r="AE13">
+        <v>6.4048319999999992E-4</v>
+      </c>
+      <c r="AF13">
+        <v>3</v>
+      </c>
+      <c r="AG13">
+        <v>2.7529791693866939E-3</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI13">
+        <v>1864341</v>
+      </c>
+      <c r="AJ13">
+        <v>443625</v>
+      </c>
+      <c r="AK13">
+        <v>1419949</v>
+      </c>
+      <c r="AL13">
+        <v>19332</v>
+      </c>
+      <c r="AM13">
+        <v>10482</v>
+      </c>
+      <c r="AN13">
+        <v>29814</v>
+      </c>
+      <c r="AO13">
+        <v>5.1154625343798217E-4</v>
+      </c>
+      <c r="AP13">
+        <v>3.0048922310418461E-3</v>
+      </c>
+      <c r="AQ13">
+        <v>-1.967E-3</v>
+      </c>
+      <c r="AR13">
+        <v>-8.9499999999999996E-4</v>
+      </c>
+      <c r="AS13">
+        <v>-1.2E-5</v>
+      </c>
+      <c r="AT13">
+        <v>1.14E-3</v>
+      </c>
+      <c r="AU13">
+        <v>8.83E-4</v>
+      </c>
+      <c r="AV13">
+        <v>-1.9059999999999999E-3</v>
+      </c>
+      <c r="AW13">
+        <v>-8.9099999999999997E-4</v>
+      </c>
+      <c r="AX13">
+        <v>-2.5999999999999998E-5</v>
+      </c>
+      <c r="AY13">
+        <v>9.990000000000001E-4</v>
+      </c>
+      <c r="AZ13">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="BA13">
+        <v>-4.3965955795592231E-4</v>
+      </c>
+      <c r="BB13">
+        <v>9.1765972312889794E-4</v>
+      </c>
+      <c r="BC13">
+        <v>429800.46413673199</v>
+      </c>
+      <c r="BD13">
+        <v>4.8320827383672276</v>
+      </c>
+      <c r="BE13">
+        <v>4.6586754945709217E-3</v>
+      </c>
+      <c r="BF13">
+        <v>-4.7361841836763927E-3</v>
+      </c>
+      <c r="BG13">
+        <v>-2.9577807004548852E-4</v>
+      </c>
+      <c r="BH13">
+        <v>-0.23013242227295949</v>
+      </c>
+      <c r="BI13">
+        <v>2069637.8939207201</v>
+      </c>
+      <c r="BJ13">
+        <v>0.16397588852116249</v>
+      </c>
+      <c r="BK13">
+        <v>1.9871120557718951</v>
+      </c>
+      <c r="BL13" t="s">
+        <v>118</v>
+      </c>
+      <c r="BM13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14">
+        <v>1903097</v>
+      </c>
+      <c r="E14">
+        <v>2E-3</v>
+      </c>
+      <c r="F14">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <v>8085</v>
+      </c>
+      <c r="H14">
+        <v>4.2483383663575744E-3</v>
+      </c>
+      <c r="I14">
+        <v>0.99575166163364237</v>
+      </c>
+      <c r="J14">
+        <v>1895012</v>
+      </c>
+      <c r="K14">
+        <v>38.013365999999998</v>
+      </c>
+      <c r="L14">
+        <v>0.129138287982</v>
+      </c>
+      <c r="M14">
+        <v>1872517</v>
+      </c>
+      <c r="N14">
+        <v>28.128403000000009</v>
+      </c>
+      <c r="O14">
+        <v>0.10202208558299999</v>
+      </c>
+      <c r="P14">
+        <v>-2.728E-3</v>
+      </c>
+      <c r="Q14">
+        <v>3.6210000000000001E-3</v>
+      </c>
+      <c r="R14">
+        <v>2.0059696719598608E-5</v>
+      </c>
+      <c r="S14">
+        <v>1.5E-5</v>
+      </c>
+      <c r="T14">
+        <v>2.6104869714726862E-4</v>
+      </c>
+      <c r="U14">
+        <v>2.6027683502341119E-4</v>
+      </c>
+      <c r="V14">
+        <v>1.9214100491184231E-4</v>
+      </c>
+      <c r="W14">
+        <v>2.2090740000000001E-4</v>
+      </c>
+      <c r="X14">
+        <v>-7.6000000000000004E-4</v>
+      </c>
+      <c r="Y14">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="Z14">
+        <v>1.502170768009049E-5</v>
+      </c>
+      <c r="AA14">
+        <v>1.4E-5</v>
+      </c>
+      <c r="AB14">
+        <v>2.3341793039583091E-4</v>
+      </c>
+      <c r="AC14">
+        <v>2.3293406476650611E-4</v>
+      </c>
+      <c r="AD14">
+        <v>1.817425406551716E-4</v>
+      </c>
+      <c r="AE14">
+        <v>2.1794220000000001E-4</v>
+      </c>
+      <c r="AF14">
+        <v>3</v>
+      </c>
+      <c r="AG14">
+        <v>7.8083050507023373E-4</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI14">
+        <v>1872517</v>
+      </c>
+      <c r="AJ14">
+        <v>983666</v>
+      </c>
+      <c r="AK14">
+        <v>885317</v>
+      </c>
+      <c r="AL14">
+        <v>15652</v>
+      </c>
+      <c r="AM14">
+        <v>6843</v>
+      </c>
+      <c r="AN14">
+        <v>22495</v>
+      </c>
+      <c r="AO14">
+        <v>4.3942933985330069E-4</v>
+      </c>
+      <c r="AP14">
+        <v>1.006148239681891E-3</v>
+      </c>
+      <c r="AQ14">
+        <v>-3.8299999999999999E-4</v>
+      </c>
+      <c r="AR14">
+        <v>-1.3300000000000001E-4</v>
+      </c>
+      <c r="AS14">
+        <v>1.65E-4</v>
+      </c>
+      <c r="AT14">
+        <v>4.2700000000000002E-4</v>
+      </c>
+      <c r="AU14">
+        <v>2.9799999999999998E-4</v>
+      </c>
+      <c r="AV14">
+        <v>-3.7500000000000001E-4</v>
+      </c>
+      <c r="AW14">
+        <v>-1.3200000000000001E-4</v>
+      </c>
+      <c r="AX14">
         <v>1.6100000000000001E-4</v>
       </c>
-      <c r="AT9">
-        <v>1.101E-3</v>
-      </c>
-      <c r="AU9">
-        <v>7.9600000000000005E-4</v>
-      </c>
-      <c r="AV9">
-        <v>-1.518E-3</v>
-      </c>
-      <c r="AW9">
-        <v>-6.2E-4</v>
-      </c>
-      <c r="AX9">
-        <v>1.5899999999999999E-4</v>
-      </c>
-      <c r="AY9">
-        <v>1.0560000000000001E-3</v>
-      </c>
-      <c r="AZ9">
-        <v>7.7899999999999996E-4</v>
-      </c>
-      <c r="BA9">
-        <v>-2.4772115611633948E-4</v>
-      </c>
-      <c r="BB9">
-        <v>8.1488061582262784E-4</v>
-      </c>
-      <c r="BC9">
-        <v>578540.15135124186</v>
-      </c>
-      <c r="BD9">
-        <v>5.2652448874361362</v>
-      </c>
-      <c r="BE9">
-        <v>4.3633475494600157E-3</v>
-      </c>
-      <c r="BF9">
-        <v>-4.2896485267772157E-3</v>
-      </c>
-      <c r="BG9">
-        <v>-9.7404824018398374E-5</v>
-      </c>
-      <c r="BH9">
-        <v>-0.28937373573272951</v>
-      </c>
-      <c r="BI9">
-        <v>1560315349.7288761</v>
-      </c>
-      <c r="BJ9">
-        <v>-0.17371904743128719</v>
-      </c>
-      <c r="BK9">
-        <v>2.0872163460411568</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>103</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>104</v>
+      <c r="AY14">
+        <v>4.0400000000000001E-4</v>
+      </c>
+      <c r="AZ14">
+        <v>2.9300000000000002E-4</v>
+      </c>
+      <c r="BA14">
+        <v>2.0059696719598608E-5</v>
+      </c>
+      <c r="BB14">
+        <v>2.6027683502341119E-4</v>
+      </c>
+      <c r="BC14">
+        <v>183021078165119.59</v>
+      </c>
+      <c r="BD14">
+        <v>9.0099222905909393</v>
+      </c>
+      <c r="BE14">
+        <v>2.8651360704615701E-3</v>
+      </c>
+      <c r="BF14">
+        <v>-2.7281138731280819E-3</v>
+      </c>
+      <c r="BG14">
+        <v>9.9854398989178417E-5</v>
+      </c>
+      <c r="BH14">
+        <v>-0.59116731166909386</v>
+      </c>
+      <c r="BI14">
+        <v>13436873327099.32</v>
+      </c>
+      <c r="BJ14">
+        <v>0.38037273959796508</v>
+      </c>
+      <c r="BK14">
+        <v>4.4904378217091372</v>
+      </c>
+      <c r="BL14" t="s">
+        <v>122</v>
+      </c>
+      <c r="BM14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:65" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2207118</v>
+      </c>
+      <c r="E15" s="15">
+        <v>2E-3</v>
+      </c>
+      <c r="F15" s="15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G15" s="15">
+        <v>256109</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0.1160377469623282</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.88396225303767173</v>
+      </c>
+      <c r="J15" s="15">
+        <v>1951009</v>
+      </c>
+      <c r="K15" s="15">
+        <v>705.81397500000003</v>
+      </c>
+      <c r="L15" s="15">
+        <v>1.601535892829</v>
+      </c>
+      <c r="M15" s="15">
+        <v>1917673</v>
+      </c>
+      <c r="N15" s="15">
+        <v>694.81338200000005</v>
+      </c>
+      <c r="O15" s="15">
+        <v>1.3125063655760001</v>
+      </c>
+      <c r="P15" s="15">
+        <v>-4.9480000000000001E-3</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>5.2440000000000004E-3</v>
+      </c>
+      <c r="R15" s="15">
+        <v>3.6176869250731288E-4</v>
+      </c>
+      <c r="S15" s="15">
+        <v>3.5300000000000002E-4</v>
+      </c>
+      <c r="T15" s="15">
+        <v>9.0602191325747433E-4</v>
+      </c>
+      <c r="U15" s="15">
+        <v>8.3066185684927383E-4</v>
+      </c>
+      <c r="V15" s="15">
+        <v>6.7501460680089126E-4</v>
+      </c>
+      <c r="W15" s="15">
+        <v>6.0638339999999986E-4</v>
+      </c>
+      <c r="X15" s="15">
+        <v>-2.1299999999999999E-3</v>
+      </c>
+      <c r="Y15" s="15">
+        <v>2.8530000000000001E-3</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>3.6232109541094859E-4</v>
+      </c>
+      <c r="AA15" s="15">
+        <v>3.5300000000000002E-4</v>
+      </c>
+      <c r="AB15" s="15">
+        <v>8.2730077732078814E-4</v>
+      </c>
+      <c r="AC15" s="15">
+        <v>7.4374054614212773E-4</v>
+      </c>
+      <c r="AD15" s="15">
+        <v>6.3634093299535426E-4</v>
+      </c>
+      <c r="AE15" s="15">
+        <v>5.9155739999999996E-4</v>
+      </c>
+      <c r="AF15" s="15">
+        <v>3</v>
+      </c>
+      <c r="AG15" s="15">
+        <v>2.491985570547822E-3</v>
+      </c>
+      <c r="AH15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI15" s="15">
+        <v>1917673</v>
+      </c>
+      <c r="AJ15" s="15">
+        <v>1405448</v>
+      </c>
+      <c r="AK15" s="15">
+        <v>511194</v>
+      </c>
+      <c r="AL15" s="15">
+        <v>16601</v>
+      </c>
+      <c r="AM15" s="15">
+        <v>16735</v>
+      </c>
+      <c r="AN15" s="15">
+        <v>33336</v>
+      </c>
+      <c r="AO15" s="15">
+        <v>3.2999139068874478E-4</v>
+      </c>
+      <c r="AP15" s="15">
+        <v>2.9259695631166662E-3</v>
+      </c>
+      <c r="AQ15" s="15">
+        <v>-9.9200000000000004E-4</v>
+      </c>
+      <c r="AR15" s="15">
+        <v>-4.1E-5</v>
+      </c>
+      <c r="AS15" s="15">
+        <v>7.7800000000000005E-4</v>
+      </c>
+      <c r="AT15" s="15">
+        <v>1.702E-3</v>
+      </c>
+      <c r="AU15" s="15">
+        <v>8.1900000000000007E-4</v>
+      </c>
+      <c r="AV15" s="15">
+        <v>-8.9700000000000001E-4</v>
+      </c>
+      <c r="AW15" s="15">
+        <v>-3.1999999999999999E-5</v>
+      </c>
+      <c r="AX15" s="15">
+        <v>7.6800000000000002E-4</v>
+      </c>
+      <c r="AY15" s="15">
+        <v>1.6130000000000001E-3</v>
+      </c>
+      <c r="AZ15" s="15">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="BA15" s="15">
+        <v>3.6176869250731288E-4</v>
+      </c>
+      <c r="BB15" s="15">
+        <v>8.3066185684927383E-4</v>
+      </c>
+      <c r="BC15" s="15">
+        <v>5272408.3306880752</v>
+      </c>
+      <c r="BD15" s="15">
+        <v>6.5165711474849974</v>
+      </c>
+      <c r="BE15" s="15">
+        <v>5.6582118115293383E-3</v>
+      </c>
+      <c r="BF15" s="15">
+        <v>-4.9483609668643912E-3</v>
+      </c>
+      <c r="BG15" s="15">
+        <v>5.6703565890667794E-4</v>
+      </c>
+      <c r="BH15" s="15">
+        <v>-0.42261579673907212</v>
+      </c>
+      <c r="BI15" s="15">
+        <v>5216161191.0168467</v>
+      </c>
+      <c r="BJ15" s="15">
+        <v>-5.6562609466715021E-2</v>
+      </c>
+      <c r="BK15" s="15">
+        <v>2.468868004107875</v>
+      </c>
+      <c r="BL15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="BM15" s="15" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2581,17 +3855,17 @@
     </sortState>
   </autoFilter>
   <mergeCells count="9">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="AV1:AZ1"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="BA1:BK1"/>
     <mergeCell ref="P1:W1"/>
     <mergeCell ref="AF1:AP1"/>
     <mergeCell ref="AQ1:AU1"/>
     <mergeCell ref="G1:L1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="AV1:AZ1"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance Multi-Illumination Processing and Reporting
- Updated orchestration log to include detailed scanning and reporting steps for distance files, including the creation of various plots and PDFs.
- Modified the Excel file for M3C2 statistics to reflect recent changes.
- Refactored the file renaming script to remove "_validonly" from filenames.
- Expanded the PlotService class to improve plotting functionality, including:
  - Added methods for reordering data and generating color mappings by case.
  - Implemented a new method to scan distance files by index, categorizing them into WITH and INLIER cases.
  - Enhanced plotting methods to support dual grouped bar plots for means and standard deviations.
  - Improved logging for better traceability during plotting and data loading processes.
</commit_message>
<xml_diff>
--- a/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
@@ -258,9 +258,6 @@
     <t>data\Multi-Illumination</t>
   </si>
   <si>
-    <t>1-1_cloud-2-1_cloud</t>
-  </si>
-  <si>
     <t>rmse</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>2025-08-28 09:46:43</t>
   </si>
   <si>
-    <t>1-2_cloud-2-2_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-2_cloud-2-2_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -285,9 +279,6 @@
     <t>2025-08-28 09:49:16</t>
   </si>
   <si>
-    <t>1-3_cloud-2-3_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-3_cloud-2-3_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>2025-08-28 09:52:36</t>
   </si>
   <si>
-    <t>1-4_cloud-2-4_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-4_cloud-2-4_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -309,9 +297,6 @@
     <t>2025-08-28 09:55:49</t>
   </si>
   <si>
-    <t>1-5_cloud-2-5_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-5_cloud-2-5_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -321,9 +306,6 @@
     <t>2025-08-28 09:59:23</t>
   </si>
   <si>
-    <t>1-6_cloud-2-6_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-6_cloud-2-6_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -333,9 +315,6 @@
     <t>2025-08-28 10:03:21</t>
   </si>
   <si>
-    <t>1-7_cloud-2-7_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-7_cloud-2-7_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -345,9 +324,6 @@
     <t>2025-08-28 10:05:50</t>
   </si>
   <si>
-    <t>1-1_cloud-2-1-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-1_cloud-2-1-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -357,9 +333,6 @@
     <t>2025-08-28 10:08:48</t>
   </si>
   <si>
-    <t>1-2_cloud-2-2-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-2_cloud-2-2-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -369,9 +342,6 @@
     <t>2025-08-28 10:11:45</t>
   </si>
   <si>
-    <t>1-3_cloud-2-3-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-3_cloud-2-3-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -381,9 +351,6 @@
     <t>2025-08-28 10:15:37</t>
   </si>
   <si>
-    <t>1-4_cloud-2-4-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-4_cloud-2-4-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -393,9 +360,6 @@
     <t>2025-08-28 10:19:20</t>
   </si>
   <si>
-    <t>1-5_cloud-2-5-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-5_cloud-2-5-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -405,9 +369,6 @@
     <t>2025-08-28 10:24:08</t>
   </si>
   <si>
-    <t>1-6_cloud-2-6-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-6_cloud-2-6-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -417,9 +378,6 @@
     <t>2025-08-28 10:29:11</t>
   </si>
   <si>
-    <t>1-7_cloud-2-7-AI_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-7_cloud-2-7-AI_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -429,9 +387,6 @@
     <t>2025-08-28 10:32:10</t>
   </si>
   <si>
-    <t>1-1-AI_cloud-2-1_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-1-AI_cloud-2-1_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -441,9 +396,6 @@
     <t>2025-08-28 10:35:42</t>
   </si>
   <si>
-    <t>1-2-AI_cloud-2-2_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-2-AI_cloud-2-2_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -453,9 +405,6 @@
     <t>2025-08-28 10:38:52</t>
   </si>
   <si>
-    <t>1-3-AI_cloud-2-3_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-3-AI_cloud-2-3_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -465,9 +414,6 @@
     <t>2025-08-28 10:43:02</t>
   </si>
   <si>
-    <t>1-4-AI_cloud-2-4_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-4-AI_cloud-2-4_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -477,9 +423,6 @@
     <t>2025-08-28 10:46:50</t>
   </si>
   <si>
-    <t>1-5-AI_cloud-2-5_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-5-AI_cloud-2-5_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -489,9 +432,6 @@
     <t>2025-08-28 10:50:31</t>
   </si>
   <si>
-    <t>1-6-AI_cloud-2-6_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-6-AI_cloud-2-6_cloud_m3c2_distances.txt</t>
   </si>
   <si>
@@ -501,13 +441,73 @@
     <t>2025-08-28 10:55:31</t>
   </si>
   <si>
-    <t>1-7-AI_cloud-2-7_cloud</t>
-  </si>
-  <si>
     <t>data\Multi-Illumination\python_1-7-AI_cloud-2-7_cloud_m3c2_distances.txt</t>
   </si>
   <si>
     <t>data\Multi-Illumination\python_1-7-AI_cloud-2-7_cloud_m3c2_params.txt</t>
+  </si>
+  <si>
+    <t>1-1 vs. 2-1</t>
+  </si>
+  <si>
+    <t>1-2 vs. 2-2</t>
+  </si>
+  <si>
+    <t>1-3 vs. 2-3</t>
+  </si>
+  <si>
+    <t>1-4 vs. 2-4</t>
+  </si>
+  <si>
+    <t>1-5 vs. 2-5</t>
+  </si>
+  <si>
+    <t>1-6 vs. 2-6</t>
+  </si>
+  <si>
+    <t>1-7 vs. 2-7</t>
+  </si>
+  <si>
+    <t>1-1 vs. 2-1-AI</t>
+  </si>
+  <si>
+    <t>1-2 vs. 2-2-AI</t>
+  </si>
+  <si>
+    <t>1-3 vs. 2-3-AI</t>
+  </si>
+  <si>
+    <t>1-4 vs. 2-4-AI</t>
+  </si>
+  <si>
+    <t>1-5 vs. 2-5-AI</t>
+  </si>
+  <si>
+    <t>1-6 vs. 2-6-AI</t>
+  </si>
+  <si>
+    <t>1-7 vs. 2-7-AI</t>
+  </si>
+  <si>
+    <t>1-1-AI vs. 2-1</t>
+  </si>
+  <si>
+    <t>1-2-AI vs. 2-2</t>
+  </si>
+  <si>
+    <t>1-3-AI vs. 2-3</t>
+  </si>
+  <si>
+    <t>1-4-AI vs. 2-4</t>
+  </si>
+  <si>
+    <t>1-5-AI vs. 2-5</t>
+  </si>
+  <si>
+    <t>1-6-AI vs. 2-6</t>
+  </si>
+  <si>
+    <t>1-7-AI vs. 2-7</t>
   </si>
 </sst>
 </file>
@@ -707,11 +707,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -721,13 +728,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1034,17 +1034,17 @@
   <dimension ref="A1:BM23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="12" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="12" customWidth="1"/>
     <col min="5" max="6" width="7.28515625" style="12" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
@@ -1087,83 +1087,83 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="19" t="s">
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="15" t="s">
+      <c r="N1" s="17"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="18" t="s">
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="21" t="s">
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="22" t="s">
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="16"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="19" t="s">
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="18"/>
+      <c r="AV1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="16"/>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="15" t="s">
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="18"/>
+      <c r="BA1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="BB1" s="16"/>
-      <c r="BC1" s="16"/>
-      <c r="BD1" s="16"/>
-      <c r="BE1" s="16"/>
-      <c r="BF1" s="16"/>
-      <c r="BG1" s="16"/>
-      <c r="BH1" s="16"/>
-      <c r="BI1" s="16"/>
-      <c r="BJ1" s="16"/>
-      <c r="BK1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="18"/>
     </row>
     <row r="2" spans="1:65" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1370,7 +1370,7 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="D3">
         <v>1848754</v>
@@ -1384,10 +1384,10 @@
       <c r="G3">
         <v>7</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="15">
         <v>3.7863339308528882E-6</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="15">
         <v>0.99999621366606917</v>
       </c>
       <c r="J3">
@@ -1463,7 +1463,7 @@
         <v>9.8928871191127001E-4</v>
       </c>
       <c r="AH3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI3">
         <v>1831404</v>
@@ -1553,21 +1553,21 @@
         <v>5.5826908358251721</v>
       </c>
       <c r="BL3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM3" t="s">
         <v>80</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="D4">
         <v>1878902</v>
@@ -1581,10 +1581,10 @@
       <c r="G4">
         <v>19318</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="15">
         <v>1.028153676987943E-2</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="15">
         <v>0.98971846323012058</v>
       </c>
       <c r="J4">
@@ -1660,7 +1660,7 @@
         <v>7.9028795658713327E-4</v>
       </c>
       <c r="AH4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI4">
         <v>1844485</v>
@@ -1750,21 +1750,21 @@
         <v>2.3040924856517102</v>
       </c>
       <c r="BL4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="BM4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>1900069</v>
@@ -1778,10 +1778,10 @@
       <c r="G5">
         <v>2215</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="15">
         <v>1.165747138656543E-3</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="15">
         <v>0.99883425286134342</v>
       </c>
       <c r="J5">
@@ -1857,7 +1857,7 @@
         <v>7.6724088045318473E-4</v>
       </c>
       <c r="AH5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI5">
         <v>1876383</v>
@@ -1947,21 +1947,21 @@
         <v>3.5078761855336662</v>
       </c>
       <c r="BL5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="BM5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>144</v>
       </c>
       <c r="D6">
         <v>1801484</v>
@@ -1975,10 +1975,10 @@
       <c r="G6">
         <v>39618</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="15">
         <v>2.1991868925841141E-2</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="15">
         <v>0.97800813107415885</v>
       </c>
       <c r="J6">
@@ -2054,7 +2054,7 @@
         <v>1.0528090686832831E-3</v>
       </c>
       <c r="AH6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI6">
         <v>1742560</v>
@@ -2144,21 +2144,21 @@
         <v>2.7922655953202851</v>
       </c>
       <c r="BL6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BM6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>145</v>
       </c>
       <c r="D7">
         <v>1838147</v>
@@ -2172,10 +2172,10 @@
       <c r="G7">
         <v>51530</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="15">
         <v>2.803366651306996E-2</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="15">
         <v>0.97196633348693007</v>
       </c>
       <c r="J7">
@@ -2251,7 +2251,7 @@
         <v>7.3150722384390289E-4</v>
       </c>
       <c r="AH7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI7">
         <v>1768833</v>
@@ -2341,21 +2341,21 @@
         <v>2.8625284060168981</v>
       </c>
       <c r="BL7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="BM7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="D8">
         <v>1843820</v>
@@ -2369,10 +2369,10 @@
       <c r="G8">
         <v>55208</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="15">
         <v>2.9942185245848289E-2</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="15">
         <v>0.97005781475415176</v>
       </c>
       <c r="J8">
@@ -2448,7 +2448,7 @@
         <v>8.4474357392821746E-4</v>
       </c>
       <c r="AH8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI8">
         <v>1763022</v>
@@ -2538,21 +2538,21 @@
         <v>5.7173596232498296</v>
       </c>
       <c r="BL8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="BM8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="D9">
         <v>1796164</v>
@@ -2566,10 +2566,10 @@
       <c r="G9">
         <v>44259</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="15">
         <v>2.464084571342038E-2</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="15">
         <v>0.9753591542865796</v>
       </c>
       <c r="J9">
@@ -2645,7 +2645,7 @@
         <v>1.0148850661627299E-3</v>
       </c>
       <c r="AH9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI9">
         <v>1736277</v>
@@ -2735,21 +2735,21 @@
         <v>2.9929042271556292</v>
       </c>
       <c r="BL9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="BM9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="D10">
         <v>1848754</v>
@@ -2763,10 +2763,10 @@
       <c r="G10">
         <v>3353</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="15">
         <v>1.8136539528785329E-3</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="15">
         <v>0.99818634604712142</v>
       </c>
       <c r="J10">
@@ -2842,7 +2842,7 @@
         <v>2.8031997153512081E-3</v>
       </c>
       <c r="AH10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI10">
         <v>1825744</v>
@@ -2932,21 +2932,21 @@
         <v>1.312988890863815</v>
       </c>
       <c r="BL10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="BM10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="D11">
         <v>1878902</v>
@@ -2960,10 +2960,10 @@
       <c r="G11">
         <v>10479</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="15">
         <v>5.5771934885374547E-3</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="15">
         <v>0.99442280651146253</v>
       </c>
       <c r="J11">
@@ -3039,7 +3039,7 @@
         <v>2.4580870792740481E-3</v>
       </c>
       <c r="AH11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI11">
         <v>1839205</v>
@@ -3129,21 +3129,21 @@
         <v>3.887307118836608</v>
       </c>
       <c r="BL11" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="BM11" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="D12">
         <v>1900069</v>
@@ -3157,10 +3157,10 @@
       <c r="G12">
         <v>2846</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="15">
         <v>1.4978403415875951E-3</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="15">
         <v>0.99850215965841238</v>
       </c>
       <c r="J12">
@@ -3236,7 +3236,7 @@
         <v>2.735073497487851E-3</v>
       </c>
       <c r="AH12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI12">
         <v>1872005</v>
@@ -3326,21 +3326,21 @@
         <v>2.4881984741804999</v>
       </c>
       <c r="BL12" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="BM12" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
       <c r="D13">
         <v>1801484</v>
@@ -3354,10 +3354,10 @@
       <c r="G13">
         <v>56184</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="15">
         <v>3.1187620872569509E-2</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="15">
         <v>0.96881237912743046</v>
       </c>
       <c r="J13">
@@ -3433,7 +3433,7 @@
         <v>2.5742086266146991E-3</v>
       </c>
       <c r="AH13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI13">
         <v>1724339</v>
@@ -3523,21 +3523,21 @@
         <v>2.320843251581115</v>
       </c>
       <c r="BL13" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="BM13" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
         <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="D14">
         <v>1838147</v>
@@ -3551,10 +3551,10 @@
       <c r="G14">
         <v>64626</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="15">
         <v>3.5158232720234023E-2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="15">
         <v>0.964841767279766</v>
       </c>
       <c r="J14">
@@ -3630,7 +3630,7 @@
         <v>2.9001213709650151E-3</v>
       </c>
       <c r="AH14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI14">
         <v>1752460</v>
@@ -3720,21 +3720,21 @@
         <v>0.98557489212421912</v>
       </c>
       <c r="BL14" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="BM14" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="D15">
         <v>1843820</v>
@@ -3748,10 +3748,10 @@
       <c r="G15">
         <v>66023</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="15">
         <v>3.5807725266023799E-2</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="15">
         <v>0.96419227473397617</v>
       </c>
       <c r="J15">
@@ -3827,7 +3827,7 @@
         <v>2.8038046472131802E-3</v>
       </c>
       <c r="AH15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI15">
         <v>1740357</v>
@@ -3917,21 +3917,21 @@
         <v>1.9910583482962569</v>
       </c>
       <c r="BL15" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="BM15" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="D16">
         <v>1796164</v>
@@ -3945,10 +3945,10 @@
       <c r="G16">
         <v>56884</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="15">
         <v>3.1669713901403211E-2</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="15">
         <v>0.96833028609859684</v>
       </c>
       <c r="J16">
@@ -4024,7 +4024,7 @@
         <v>2.2744475866410571E-3</v>
       </c>
       <c r="AH16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI16">
         <v>1717687</v>
@@ -4114,21 +4114,21 @@
         <v>1.99486544504208</v>
       </c>
       <c r="BL16" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="BM16" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
         <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D17">
         <v>2143284</v>
@@ -4142,10 +4142,10 @@
       <c r="G17">
         <v>214008</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="15">
         <v>9.9850509778452126E-2</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I17" s="15">
         <v>0.90014949022154789</v>
       </c>
       <c r="J17">
@@ -4221,7 +4221,7 @@
         <v>3.3627550205738588E-3</v>
       </c>
       <c r="AH17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI17">
         <v>1917090</v>
@@ -4311,21 +4311,21 @@
         <v>0.9798550044227512</v>
       </c>
       <c r="BL17" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="BM17" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
         <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="D18">
         <v>2205767</v>
@@ -4339,10 +4339,10 @@
       <c r="G18">
         <v>292676</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="15">
         <v>0.13268672529782161</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="15">
         <v>0.86731327470217845</v>
       </c>
       <c r="J18">
@@ -4418,7 +4418,7 @@
         <v>2.8114752880003539E-3</v>
       </c>
       <c r="AH18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI18">
         <v>1889709</v>
@@ -4508,21 +4508,21 @@
         <v>2.4033292130696382</v>
       </c>
       <c r="BL18" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="BM18" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D19">
         <v>2205244</v>
@@ -4536,10 +4536,10 @@
       <c r="G19">
         <v>268241</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="15">
         <v>0.1216377870203932</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="15">
         <v>0.87836221297960682</v>
       </c>
       <c r="J19">
@@ -4615,7 +4615,7 @@
         <v>3.076050921849162E-3</v>
       </c>
       <c r="AH19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI19">
         <v>1918919</v>
@@ -4705,21 +4705,21 @@
         <v>2.141493775871214</v>
       </c>
       <c r="BL19" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="BM19" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
         <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D20">
         <v>2077959</v>
@@ -4733,10 +4733,10 @@
       <c r="G20">
         <v>205403</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="15">
         <v>9.8848437336829076E-2</v>
       </c>
-      <c r="I20" s="23">
+      <c r="I20" s="15">
         <v>0.90115156266317098</v>
       </c>
       <c r="J20">
@@ -4812,7 +4812,7 @@
         <v>2.7153590076049688E-3</v>
       </c>
       <c r="AH20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI20">
         <v>1846119</v>
@@ -4902,21 +4902,21 @@
         <v>2.8173133865784599</v>
       </c>
       <c r="BL20" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="BM20" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D21">
         <v>2117896</v>
@@ -4930,10 +4930,10 @@
       <c r="G21">
         <v>231482</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="15">
         <v>0.1092980958460661</v>
       </c>
-      <c r="I21" s="23">
+      <c r="I21" s="15">
         <v>0.89070190415393391</v>
       </c>
       <c r="J21">
@@ -5009,7 +5009,7 @@
         <v>3.034097210630938E-3</v>
       </c>
       <c r="AH21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI21">
         <v>1862944</v>
@@ -5099,21 +5099,21 @@
         <v>2.9706067384547929</v>
       </c>
       <c r="BL21" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="BM21" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D22">
         <v>2121774</v>
@@ -5127,10 +5127,10 @@
       <c r="G22">
         <v>237602</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="15">
         <v>0.111982708808761</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="15">
         <v>0.88801729119123907</v>
       </c>
       <c r="J22">
@@ -5206,7 +5206,7 @@
         <v>2.691529972437468E-3</v>
       </c>
       <c r="AH22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI22">
         <v>1858004</v>
@@ -5296,21 +5296,21 @@
         <v>2.628172273098841</v>
       </c>
       <c r="BL22" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="BM22" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D23">
         <v>2070938</v>
@@ -5324,10 +5324,10 @@
       <c r="G23">
         <v>215645</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="15">
         <v>0.10412914341230881</v>
       </c>
-      <c r="I23" s="23">
+      <c r="I23" s="15">
         <v>0.89587085658769117</v>
       </c>
       <c r="J23">
@@ -5403,7 +5403,7 @@
         <v>2.864988469496788E-3</v>
       </c>
       <c r="AH23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AI23">
         <v>1834386</v>
@@ -5493,10 +5493,10 @@
         <v>2.5450449789946501</v>
       </c>
       <c r="BL23" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="BM23" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5506,6 +5506,8 @@
     </sortState>
   </autoFilter>
   <mergeCells count="9">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="BA1:BK1"/>
     <mergeCell ref="P1:W1"/>
     <mergeCell ref="AF1:AP1"/>
@@ -5513,8 +5515,6 @@
     <mergeCell ref="G1:L1"/>
     <mergeCell ref="X1:AE1"/>
     <mergeCell ref="AV1:AZ1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add logging for Multi-Illumination processing and fix outlier exclusion error
- Enhanced orchestration.log with detailed logs for Multi-Illumination processing, including job configurations, point cloud readings, and run statistics.
- Fixed a TypeError in the outlier exclusion function by addressing the unexpected keyword argument 'data_folder'.
- Updated py4dgeo.log to include additional logs for point cloud readings and KDTree structure building during Multi-Illumination processing.
- Updated binary output file MARS_Multi_Illumination_m3c2_stats_distances.xlsx to reflect changes in processing results.
</commit_message>
<xml_diff>
--- a/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
@@ -618,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM27"/>
+  <dimension ref="A1:BM31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -6328,6 +6328,842 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-09-01 09:25:46</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>a-1-b-1</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1848754</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G28" t="n">
+        <v>7</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3.786333930852888e-06</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.9999962136660692</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1848747</v>
+      </c>
+      <c r="K28" t="n">
+        <v>58.06580200000001</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.201039354048</v>
+      </c>
+      <c r="M28" t="n">
+        <v>1831404</v>
+      </c>
+      <c r="N28" t="n">
+        <v>64.48812999999998</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.16406526557</v>
+      </c>
+      <c r="P28" t="n">
+        <v>-0.004257</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.004802</v>
+      </c>
+      <c r="R28" t="n">
+        <v>3.140819268401788e-05</v>
+      </c>
+      <c r="S28" t="n">
+        <v>4.4e-05</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.0003297629039704233</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0.0003282637632565164</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.0002423816000783233</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.0002683506</v>
+      </c>
+      <c r="X28" t="n">
+        <v>-0.0009890000000000001</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.0009890000000000001</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>3.521239988555228e-05</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>4.5e-05</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.000299306565652362</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.0002972280389480636</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.0002315634911794449</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.0002653854</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.00098928871191127</v>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI28" t="n">
+        <v>1831404</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>1041360</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>787214</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>6541</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>10802</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>17343</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>-0.0003703124026984951</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>0.001412373977284256</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>-0.000513</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>-0.000141</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>0.000222</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>0.000523</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>0.000363</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>-0.000491</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>-0.000137</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>0.000221</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>0.000513</v>
+      </c>
+      <c r="AZ28" t="n">
+        <v>0.000358</v>
+      </c>
+      <c r="BA28" t="n">
+        <v>3.140819268401788e-05</v>
+      </c>
+      <c r="BB28" t="n">
+        <v>0.0003282637632565164</v>
+      </c>
+      <c r="BC28" t="n">
+        <v>1127175200681164</v>
+      </c>
+      <c r="BD28" t="n">
+        <v>12.22131184167564</v>
+      </c>
+      <c r="BE28" t="n">
+        <v>0.00443167676357952</v>
+      </c>
+      <c r="BF28" t="n">
+        <v>-0.004257395391128698</v>
+      </c>
+      <c r="BG28" t="n">
+        <v>0.0001434337456783985</v>
+      </c>
+      <c r="BH28" t="n">
+        <v>-0.7175292079112111</v>
+      </c>
+      <c r="BI28" t="n">
+        <v>14923656066230.08</v>
+      </c>
+      <c r="BJ28" t="n">
+        <v>-0.5887868609417466</v>
+      </c>
+      <c r="BK28" t="n">
+        <v>5.582690835825172</v>
+      </c>
+      <c r="BL28" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-b-1_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM28" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-b-1_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-09-01 09:27:16</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>a-1-b-1-AI</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1848754</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3353</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.001813653952878533</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.9981863460471214</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1845401</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-671.42272</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1.611225486426</v>
+      </c>
+      <c r="M29" t="n">
+        <v>1825744</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-626.261582</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1.407286543668</v>
+      </c>
+      <c r="P29" t="n">
+        <v>-0.00432</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.004148</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-0.0003638356758233035</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-0.000283</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0.0009343999051170693</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0.0008606548574666783</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.0006962032219555533</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.000748713</v>
+      </c>
+      <c r="X29" t="n">
+        <v>-0.002803</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.002803</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>-0.0003430171929909122</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>-0.000275</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0.0008779531198573015</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.0008081713221711127</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.0006691691233820295</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.0007383347999999999</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0.002803199715351208</v>
+      </c>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI29" t="n">
+        <v>1825744</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>624201</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>1200506</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>2784</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>16873</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>19657</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>-0.002297458310016787</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>0.002257556550696858</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>-0.001857</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>-0.000859</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>0.00017</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>0.000891</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>0.001029</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>-0.00177</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>-0.00084</v>
+      </c>
+      <c r="AX29" t="n">
+        <v>0.000172</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>0.000882</v>
+      </c>
+      <c r="AZ29" t="n">
+        <v>0.001012</v>
+      </c>
+      <c r="BA29" t="n">
+        <v>-0.0003638356758233035</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>0.0008606548574666783</v>
+      </c>
+      <c r="BC29" t="n">
+        <v>248623.2555508183</v>
+      </c>
+      <c r="BD29" t="n">
+        <v>5.100174121428031</v>
+      </c>
+      <c r="BE29" t="n">
+        <v>0.004338516079674972</v>
+      </c>
+      <c r="BF29" t="n">
+        <v>-0.004368371937607233</v>
+      </c>
+      <c r="BG29" t="n">
+        <v>-0.0002115922981897056</v>
+      </c>
+      <c r="BH29" t="n">
+        <v>-0.2677860148641807</v>
+      </c>
+      <c r="BI29" t="n">
+        <v>1326327888.537201</v>
+      </c>
+      <c r="BJ29" t="n">
+        <v>-0.2770356403359415</v>
+      </c>
+      <c r="BK29" t="n">
+        <v>1.312988890863815</v>
+      </c>
+      <c r="BL29" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-b-1-AI_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM29" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-b-1-AI_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-09-01 09:29:02</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>a-1-AI-b-1</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2143284</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G30" t="n">
+        <v>214008</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.09985050977845213</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.9001494902215479</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1929276</v>
+      </c>
+      <c r="K30" t="n">
+        <v>944.0018060000002</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2.42405412044</v>
+      </c>
+      <c r="M30" t="n">
+        <v>1917090</v>
+      </c>
+      <c r="N30" t="n">
+        <v>912.6991869999999</v>
+      </c>
+      <c r="O30" t="n">
+        <v>2.261979214093</v>
+      </c>
+      <c r="P30" t="n">
+        <v>-0.005808</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.004936</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.0004893036589891754</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.000482</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.001120918340191286</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.001008483938730307</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.0008716386053628407</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.0008776991999999999</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-0.003362</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.003362</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0.0004760857273263122</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0.000477</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0.001086233153461209</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.000976342585322621</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.000854039257937812</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.0008702861999999999</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0.003362755020573859</v>
+      </c>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI30" t="n">
+        <v>1917090</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>1367184</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>549002</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>10429</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>1757</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>12186</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>0.002568736172657148</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>0.002588761337714701</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>-0.001169</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>-9.8e-05</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>0.001086</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>0.002158</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>0.001184</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>-0.001162</v>
+      </c>
+      <c r="AW30" t="n">
+        <v>-0.0001</v>
+      </c>
+      <c r="AX30" t="n">
+        <v>0.001074</v>
+      </c>
+      <c r="AY30" t="n">
+        <v>0.002095</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>0.001174</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>0.0004893036589891754</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>0.001008483938730307</v>
+      </c>
+      <c r="BC30" t="n">
+        <v>122338.8498843068</v>
+      </c>
+      <c r="BD30" t="n">
+        <v>6.632135228644302</v>
+      </c>
+      <c r="BE30" t="n">
+        <v>0.006722693953013577</v>
+      </c>
+      <c r="BF30" t="n">
+        <v>-0.005808409162356089</v>
+      </c>
+      <c r="BG30" t="n">
+        <v>0.0007506396059552209</v>
+      </c>
+      <c r="BH30" t="n">
+        <v>-0.4327674980723418</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>203600348.2673969</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>-0.04436061331310492</v>
+      </c>
+      <c r="BK30" t="n">
+        <v>0.9798550044227512</v>
+      </c>
+      <c r="BL30" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-AI-b-1_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM30" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-AI-b-1_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-09-01 09:31:04</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>a-1-AI-b-1-AI</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2143284</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G31" t="n">
+        <v>25924</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.01209545725158215</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.9879045427484179</v>
+      </c>
+      <c r="J31" t="n">
+        <v>2117360</v>
+      </c>
+      <c r="K31" t="n">
+        <v>522.5222369999999</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1.987969683329</v>
+      </c>
+      <c r="M31" t="n">
+        <v>2067166</v>
+      </c>
+      <c r="N31" t="n">
+        <v>387.117282</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1.390636687952</v>
+      </c>
+      <c r="P31" t="n">
+        <v>-0.005688</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.00617</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.0002467800643253863</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.000183</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.000968963742060044</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.0009370113837507853</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.0006621369068084785</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.0006063833999999999</v>
+      </c>
+      <c r="X31" t="n">
+        <v>-0.002906</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.002906</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.0001872695671271683</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0.00017</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.0008201988665263999</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.0007985338376544816</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.0005949083663334245</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.0005841444</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0.002906891226180132</v>
+      </c>
+      <c r="AH31" t="inlineStr">
+        <is>
+          <t>rmse</t>
+        </is>
+      </c>
+      <c r="AI31" t="n">
+        <v>2067166</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>1281193</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>784476</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>44868</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>5326</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>50194</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>0.002697632286727497</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>0.002150178147824242</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>-0.001117</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>-0.000234</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>0.0005820000000000001</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>0.002048</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>0.0008160000000000001</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>-0.0011</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>-0.000241</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>0.000545</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>0.001659</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>0.000786</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>0.0002467800643253863</v>
+      </c>
+      <c r="BB31" t="n">
+        <v>0.0009370113837507853</v>
+      </c>
+      <c r="BC31" t="n">
+        <v>1561851.362796817</v>
+      </c>
+      <c r="BD31" t="n">
+        <v>5.939962160905105</v>
+      </c>
+      <c r="BE31" t="n">
+        <v>0.006340247401192347</v>
+      </c>
+      <c r="BF31" t="n">
+        <v>-0.005688138567817923</v>
+      </c>
+      <c r="BG31" t="n">
+        <v>0.0004583629744138711</v>
+      </c>
+      <c r="BH31" t="n">
+        <v>-0.3670612797172161</v>
+      </c>
+      <c r="BI31" t="n">
+        <v>11693423546.35915</v>
+      </c>
+      <c r="BJ31" t="n">
+        <v>0.7472737316746452</v>
+      </c>
+      <c r="BK31" t="n">
+        <v>2.994743908023999</v>
+      </c>
+      <c r="BL31" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-AI-b-1-AI_m3c2_distances.txt</t>
+        </is>
+      </c>
+      <c r="BM31" t="inlineStr">
+        <is>
+          <t>data\Multi-Illumination\python_a-1-AI-b-1-AI_m3c2_params.txt</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:BE2">
     <sortState ref="A2:BC25">

</xml_diff>

<commit_message>
Refactor service imports and update test cases
- Changed import paths for ParamEstimator and exclude_outliers to their respective service modules.
- Updated references in test files to reflect the new import paths.
- Modified orchestration script to align with the new service structure.
- Updated binary output file indicating changes in MARS Multi-Illumination statistics.
- Enhanced logging in py4dgeo.log to include additional point cloud reading events.
</commit_message>
<xml_diff>
--- a/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
+++ b/outputs/MARS_Multi_Illumination_output/MARS_Multi_Illumination_m3c2_stats_distances.xlsx
@@ -237,19 +237,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,13 +618,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM31"/>
+  <dimension ref="A1:BM27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -660,8 +660,8 @@
     <col width="10.5703125" bestFit="1" customWidth="1" style="12" min="63" max="63"/>
     <col hidden="1" width="125.42578125" customWidth="1" style="12" min="64" max="64"/>
     <col hidden="1" width="44.5703125" customWidth="1" style="12" min="65" max="65"/>
-    <col width="9.140625" customWidth="1" style="12" min="66" max="74"/>
-    <col width="9.140625" customWidth="1" style="12" min="75" max="16384"/>
+    <col width="9.140625" customWidth="1" style="12" min="66" max="75"/>
+    <col width="9.140625" customWidth="1" style="12" min="76" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="39.75" customHeight="1" s="12">
@@ -680,7 +680,7 @@
           <t>Calculated on Outliers only</t>
         </is>
       </c>
-      <c r="E1" s="23" t="inlineStr">
+      <c r="E1" s="19" t="inlineStr">
         <is>
           <t>Parameters used for Algorithm</t>
         </is>
@@ -696,7 +696,7 @@
       <c r="J1" s="17" t="n"/>
       <c r="K1" s="17" t="n"/>
       <c r="L1" s="18" t="n"/>
-      <c r="M1" s="22" t="inlineStr">
+      <c r="M1" s="20" t="inlineStr">
         <is>
           <t>exkl. Outliers</t>
         </is>
@@ -727,7 +727,7 @@
       <c r="AC1" s="17" t="n"/>
       <c r="AD1" s="17" t="n"/>
       <c r="AE1" s="17" t="n"/>
-      <c r="AF1" s="19" t="inlineStr">
+      <c r="AF1" s="22" t="inlineStr">
         <is>
           <t>Inlier / Outlier Details</t>
         </is>
@@ -742,7 +742,7 @@
       <c r="AN1" s="17" t="n"/>
       <c r="AO1" s="17" t="n"/>
       <c r="AP1" s="18" t="n"/>
-      <c r="AQ1" s="20" t="inlineStr">
+      <c r="AQ1" s="23" t="inlineStr">
         <is>
           <t>Quantiles All Points (incl. Outliers)</t>
         </is>
@@ -751,7 +751,7 @@
       <c r="AS1" s="17" t="n"/>
       <c r="AT1" s="17" t="n"/>
       <c r="AU1" s="18" t="n"/>
-      <c r="AV1" s="22" t="inlineStr">
+      <c r="AV1" s="20" t="inlineStr">
         <is>
           <t>Quantiles (excl. Outliers)</t>
         </is>
@@ -5495,7 +5495,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-08-29 08:47:12</t>
+          <t>2025-09-01 10:34:17</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -5704,7 +5704,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-08-29 08:48:48</t>
+          <t>2025-09-01 10:36:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -5913,7 +5913,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-08-29 08:50:41</t>
+          <t>2025-09-01 10:38:06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -6122,7 +6122,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-08-29 08:52:49</t>
+          <t>2025-09-01 10:41:15</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -6323,842 +6323,6 @@
         </is>
       </c>
       <c r="BM27" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-AI-b-1-AI_m3c2_params.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2025-09-01 09:25:46</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>a-1-b-1</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>1848754</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="G28" t="n">
-        <v>7</v>
-      </c>
-      <c r="H28" t="n">
-        <v>3.786333930852888e-06</v>
-      </c>
-      <c r="I28" t="n">
-        <v>0.9999962136660692</v>
-      </c>
-      <c r="J28" t="n">
-        <v>1848747</v>
-      </c>
-      <c r="K28" t="n">
-        <v>58.06580200000001</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0.201039354048</v>
-      </c>
-      <c r="M28" t="n">
-        <v>1831404</v>
-      </c>
-      <c r="N28" t="n">
-        <v>64.48812999999998</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0.16406526557</v>
-      </c>
-      <c r="P28" t="n">
-        <v>-0.004257</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0.004802</v>
-      </c>
-      <c r="R28" t="n">
-        <v>3.140819268401788e-05</v>
-      </c>
-      <c r="S28" t="n">
-        <v>4.4e-05</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0.0003297629039704233</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0.0003282637632565164</v>
-      </c>
-      <c r="V28" t="n">
-        <v>0.0002423816000783233</v>
-      </c>
-      <c r="W28" t="n">
-        <v>0.0002683506</v>
-      </c>
-      <c r="X28" t="n">
-        <v>-0.0009890000000000001</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>0.0009890000000000001</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>3.521239988555228e-05</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>4.5e-05</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>0.000299306565652362</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>0.0002972280389480636</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0.0002315634911794449</v>
-      </c>
-      <c r="AE28" t="n">
-        <v>0.0002653854</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>0.00098928871191127</v>
-      </c>
-      <c r="AH28" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="AI28" t="n">
-        <v>1831404</v>
-      </c>
-      <c r="AJ28" t="n">
-        <v>1041360</v>
-      </c>
-      <c r="AK28" t="n">
-        <v>787214</v>
-      </c>
-      <c r="AL28" t="n">
-        <v>6541</v>
-      </c>
-      <c r="AM28" t="n">
-        <v>10802</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>17343</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>-0.0003703124026984951</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>0.001412373977284256</v>
-      </c>
-      <c r="AQ28" t="n">
-        <v>-0.000513</v>
-      </c>
-      <c r="AR28" t="n">
-        <v>-0.000141</v>
-      </c>
-      <c r="AS28" t="n">
-        <v>0.000222</v>
-      </c>
-      <c r="AT28" t="n">
-        <v>0.000523</v>
-      </c>
-      <c r="AU28" t="n">
-        <v>0.000363</v>
-      </c>
-      <c r="AV28" t="n">
-        <v>-0.000491</v>
-      </c>
-      <c r="AW28" t="n">
-        <v>-0.000137</v>
-      </c>
-      <c r="AX28" t="n">
-        <v>0.000221</v>
-      </c>
-      <c r="AY28" t="n">
-        <v>0.000513</v>
-      </c>
-      <c r="AZ28" t="n">
-        <v>0.000358</v>
-      </c>
-      <c r="BA28" t="n">
-        <v>3.140819268401788e-05</v>
-      </c>
-      <c r="BB28" t="n">
-        <v>0.0003282637632565164</v>
-      </c>
-      <c r="BC28" t="n">
-        <v>1127175200681164</v>
-      </c>
-      <c r="BD28" t="n">
-        <v>12.22131184167564</v>
-      </c>
-      <c r="BE28" t="n">
-        <v>0.00443167676357952</v>
-      </c>
-      <c r="BF28" t="n">
-        <v>-0.004257395391128698</v>
-      </c>
-      <c r="BG28" t="n">
-        <v>0.0001434337456783985</v>
-      </c>
-      <c r="BH28" t="n">
-        <v>-0.7175292079112111</v>
-      </c>
-      <c r="BI28" t="n">
-        <v>14923656066230.08</v>
-      </c>
-      <c r="BJ28" t="n">
-        <v>-0.5887868609417466</v>
-      </c>
-      <c r="BK28" t="n">
-        <v>5.582690835825172</v>
-      </c>
-      <c r="BL28" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-b-1_m3c2_distances.txt</t>
-        </is>
-      </c>
-      <c r="BM28" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-b-1_m3c2_params.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2025-09-01 09:27:16</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>a-1-b-1-AI</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>1848754</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="G29" t="n">
-        <v>3353</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.001813653952878533</v>
-      </c>
-      <c r="I29" t="n">
-        <v>0.9981863460471214</v>
-      </c>
-      <c r="J29" t="n">
-        <v>1845401</v>
-      </c>
-      <c r="K29" t="n">
-        <v>-671.42272</v>
-      </c>
-      <c r="L29" t="n">
-        <v>1.611225486426</v>
-      </c>
-      <c r="M29" t="n">
-        <v>1825744</v>
-      </c>
-      <c r="N29" t="n">
-        <v>-626.261582</v>
-      </c>
-      <c r="O29" t="n">
-        <v>1.407286543668</v>
-      </c>
-      <c r="P29" t="n">
-        <v>-0.00432</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>0.004148</v>
-      </c>
-      <c r="R29" t="n">
-        <v>-0.0003638356758233035</v>
-      </c>
-      <c r="S29" t="n">
-        <v>-0.000283</v>
-      </c>
-      <c r="T29" t="n">
-        <v>0.0009343999051170693</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0.0008606548574666783</v>
-      </c>
-      <c r="V29" t="n">
-        <v>0.0006962032219555533</v>
-      </c>
-      <c r="W29" t="n">
-        <v>0.000748713</v>
-      </c>
-      <c r="X29" t="n">
-        <v>-0.002803</v>
-      </c>
-      <c r="Y29" t="n">
-        <v>0.002803</v>
-      </c>
-      <c r="Z29" t="n">
-        <v>-0.0003430171929909122</v>
-      </c>
-      <c r="AA29" t="n">
-        <v>-0.000275</v>
-      </c>
-      <c r="AB29" t="n">
-        <v>0.0008779531198573015</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>0.0008081713221711127</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>0.0006691691233820295</v>
-      </c>
-      <c r="AE29" t="n">
-        <v>0.0007383347999999999</v>
-      </c>
-      <c r="AF29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG29" t="n">
-        <v>0.002803199715351208</v>
-      </c>
-      <c r="AH29" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="AI29" t="n">
-        <v>1825744</v>
-      </c>
-      <c r="AJ29" t="n">
-        <v>624201</v>
-      </c>
-      <c r="AK29" t="n">
-        <v>1200506</v>
-      </c>
-      <c r="AL29" t="n">
-        <v>2784</v>
-      </c>
-      <c r="AM29" t="n">
-        <v>16873</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>19657</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>-0.002297458310016787</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>0.002257556550696858</v>
-      </c>
-      <c r="AQ29" t="n">
-        <v>-0.001857</v>
-      </c>
-      <c r="AR29" t="n">
-        <v>-0.000859</v>
-      </c>
-      <c r="AS29" t="n">
-        <v>0.00017</v>
-      </c>
-      <c r="AT29" t="n">
-        <v>0.000891</v>
-      </c>
-      <c r="AU29" t="n">
-        <v>0.001029</v>
-      </c>
-      <c r="AV29" t="n">
-        <v>-0.00177</v>
-      </c>
-      <c r="AW29" t="n">
-        <v>-0.00084</v>
-      </c>
-      <c r="AX29" t="n">
-        <v>0.000172</v>
-      </c>
-      <c r="AY29" t="n">
-        <v>0.000882</v>
-      </c>
-      <c r="AZ29" t="n">
-        <v>0.001012</v>
-      </c>
-      <c r="BA29" t="n">
-        <v>-0.0003638356758233035</v>
-      </c>
-      <c r="BB29" t="n">
-        <v>0.0008606548574666783</v>
-      </c>
-      <c r="BC29" t="n">
-        <v>248623.2555508183</v>
-      </c>
-      <c r="BD29" t="n">
-        <v>5.100174121428031</v>
-      </c>
-      <c r="BE29" t="n">
-        <v>0.004338516079674972</v>
-      </c>
-      <c r="BF29" t="n">
-        <v>-0.004368371937607233</v>
-      </c>
-      <c r="BG29" t="n">
-        <v>-0.0002115922981897056</v>
-      </c>
-      <c r="BH29" t="n">
-        <v>-0.2677860148641807</v>
-      </c>
-      <c r="BI29" t="n">
-        <v>1326327888.537201</v>
-      </c>
-      <c r="BJ29" t="n">
-        <v>-0.2770356403359415</v>
-      </c>
-      <c r="BK29" t="n">
-        <v>1.312988890863815</v>
-      </c>
-      <c r="BL29" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-b-1-AI_m3c2_distances.txt</t>
-        </is>
-      </c>
-      <c r="BM29" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-b-1-AI_m3c2_params.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-09-01 09:29:02</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>a-1-AI-b-1</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>2143284</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="G30" t="n">
-        <v>214008</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.09985050977845213</v>
-      </c>
-      <c r="I30" t="n">
-        <v>0.9001494902215479</v>
-      </c>
-      <c r="J30" t="n">
-        <v>1929276</v>
-      </c>
-      <c r="K30" t="n">
-        <v>944.0018060000002</v>
-      </c>
-      <c r="L30" t="n">
-        <v>2.42405412044</v>
-      </c>
-      <c r="M30" t="n">
-        <v>1917090</v>
-      </c>
-      <c r="N30" t="n">
-        <v>912.6991869999999</v>
-      </c>
-      <c r="O30" t="n">
-        <v>2.261979214093</v>
-      </c>
-      <c r="P30" t="n">
-        <v>-0.005808</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0.004936</v>
-      </c>
-      <c r="R30" t="n">
-        <v>0.0004893036589891754</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0.000482</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0.001120918340191286</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0.001008483938730307</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0.0008716386053628407</v>
-      </c>
-      <c r="W30" t="n">
-        <v>0.0008776991999999999</v>
-      </c>
-      <c r="X30" t="n">
-        <v>-0.003362</v>
-      </c>
-      <c r="Y30" t="n">
-        <v>0.003362</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>0.0004760857273263122</v>
-      </c>
-      <c r="AA30" t="n">
-        <v>0.000477</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>0.001086233153461209</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>0.000976342585322621</v>
-      </c>
-      <c r="AD30" t="n">
-        <v>0.000854039257937812</v>
-      </c>
-      <c r="AE30" t="n">
-        <v>0.0008702861999999999</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG30" t="n">
-        <v>0.003362755020573859</v>
-      </c>
-      <c r="AH30" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="AI30" t="n">
-        <v>1917090</v>
-      </c>
-      <c r="AJ30" t="n">
-        <v>1367184</v>
-      </c>
-      <c r="AK30" t="n">
-        <v>549002</v>
-      </c>
-      <c r="AL30" t="n">
-        <v>10429</v>
-      </c>
-      <c r="AM30" t="n">
-        <v>1757</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>12186</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>0.002568736172657148</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>0.002588761337714701</v>
-      </c>
-      <c r="AQ30" t="n">
-        <v>-0.001169</v>
-      </c>
-      <c r="AR30" t="n">
-        <v>-9.8e-05</v>
-      </c>
-      <c r="AS30" t="n">
-        <v>0.001086</v>
-      </c>
-      <c r="AT30" t="n">
-        <v>0.002158</v>
-      </c>
-      <c r="AU30" t="n">
-        <v>0.001184</v>
-      </c>
-      <c r="AV30" t="n">
-        <v>-0.001162</v>
-      </c>
-      <c r="AW30" t="n">
-        <v>-0.0001</v>
-      </c>
-      <c r="AX30" t="n">
-        <v>0.001074</v>
-      </c>
-      <c r="AY30" t="n">
-        <v>0.002095</v>
-      </c>
-      <c r="AZ30" t="n">
-        <v>0.001174</v>
-      </c>
-      <c r="BA30" t="n">
-        <v>0.0004893036589891754</v>
-      </c>
-      <c r="BB30" t="n">
-        <v>0.001008483938730307</v>
-      </c>
-      <c r="BC30" t="n">
-        <v>122338.8498843068</v>
-      </c>
-      <c r="BD30" t="n">
-        <v>6.632135228644302</v>
-      </c>
-      <c r="BE30" t="n">
-        <v>0.006722693953013577</v>
-      </c>
-      <c r="BF30" t="n">
-        <v>-0.005808409162356089</v>
-      </c>
-      <c r="BG30" t="n">
-        <v>0.0007506396059552209</v>
-      </c>
-      <c r="BH30" t="n">
-        <v>-0.4327674980723418</v>
-      </c>
-      <c r="BI30" t="n">
-        <v>203600348.2673969</v>
-      </c>
-      <c r="BJ30" t="n">
-        <v>-0.04436061331310492</v>
-      </c>
-      <c r="BK30" t="n">
-        <v>0.9798550044227512</v>
-      </c>
-      <c r="BL30" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-AI-b-1_m3c2_distances.txt</t>
-        </is>
-      </c>
-      <c r="BM30" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-AI-b-1_m3c2_params.txt</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2025-09-01 09:31:04</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>a-1-AI-b-1-AI</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>2143284</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="G31" t="n">
-        <v>25924</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.01209545725158215</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0.9879045427484179</v>
-      </c>
-      <c r="J31" t="n">
-        <v>2117360</v>
-      </c>
-      <c r="K31" t="n">
-        <v>522.5222369999999</v>
-      </c>
-      <c r="L31" t="n">
-        <v>1.987969683329</v>
-      </c>
-      <c r="M31" t="n">
-        <v>2067166</v>
-      </c>
-      <c r="N31" t="n">
-        <v>387.117282</v>
-      </c>
-      <c r="O31" t="n">
-        <v>1.390636687952</v>
-      </c>
-      <c r="P31" t="n">
-        <v>-0.005688</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>0.00617</v>
-      </c>
-      <c r="R31" t="n">
-        <v>0.0002467800643253863</v>
-      </c>
-      <c r="S31" t="n">
-        <v>0.000183</v>
-      </c>
-      <c r="T31" t="n">
-        <v>0.000968963742060044</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0.0009370113837507853</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0.0006621369068084785</v>
-      </c>
-      <c r="W31" t="n">
-        <v>0.0006063833999999999</v>
-      </c>
-      <c r="X31" t="n">
-        <v>-0.002906</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>0.002906</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>0.0001872695671271683</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>0.00017</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0.0008201988665263999</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>0.0007985338376544816</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>0.0005949083663334245</v>
-      </c>
-      <c r="AE31" t="n">
-        <v>0.0005841444</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AG31" t="n">
-        <v>0.002906891226180132</v>
-      </c>
-      <c r="AH31" t="inlineStr">
-        <is>
-          <t>rmse</t>
-        </is>
-      </c>
-      <c r="AI31" t="n">
-        <v>2067166</v>
-      </c>
-      <c r="AJ31" t="n">
-        <v>1281193</v>
-      </c>
-      <c r="AK31" t="n">
-        <v>784476</v>
-      </c>
-      <c r="AL31" t="n">
-        <v>44868</v>
-      </c>
-      <c r="AM31" t="n">
-        <v>5326</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>50194</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>0.002697632286727497</v>
-      </c>
-      <c r="AP31" t="n">
-        <v>0.002150178147824242</v>
-      </c>
-      <c r="AQ31" t="n">
-        <v>-0.001117</v>
-      </c>
-      <c r="AR31" t="n">
-        <v>-0.000234</v>
-      </c>
-      <c r="AS31" t="n">
-        <v>0.0005820000000000001</v>
-      </c>
-      <c r="AT31" t="n">
-        <v>0.002048</v>
-      </c>
-      <c r="AU31" t="n">
-        <v>0.0008160000000000001</v>
-      </c>
-      <c r="AV31" t="n">
-        <v>-0.0011</v>
-      </c>
-      <c r="AW31" t="n">
-        <v>-0.000241</v>
-      </c>
-      <c r="AX31" t="n">
-        <v>0.000545</v>
-      </c>
-      <c r="AY31" t="n">
-        <v>0.001659</v>
-      </c>
-      <c r="AZ31" t="n">
-        <v>0.000786</v>
-      </c>
-      <c r="BA31" t="n">
-        <v>0.0002467800643253863</v>
-      </c>
-      <c r="BB31" t="n">
-        <v>0.0009370113837507853</v>
-      </c>
-      <c r="BC31" t="n">
-        <v>1561851.362796817</v>
-      </c>
-      <c r="BD31" t="n">
-        <v>5.939962160905105</v>
-      </c>
-      <c r="BE31" t="n">
-        <v>0.006340247401192347</v>
-      </c>
-      <c r="BF31" t="n">
-        <v>-0.005688138567817923</v>
-      </c>
-      <c r="BG31" t="n">
-        <v>0.0004583629744138711</v>
-      </c>
-      <c r="BH31" t="n">
-        <v>-0.3670612797172161</v>
-      </c>
-      <c r="BI31" t="n">
-        <v>11693423546.35915</v>
-      </c>
-      <c r="BJ31" t="n">
-        <v>0.7472737316746452</v>
-      </c>
-      <c r="BK31" t="n">
-        <v>2.994743908023999</v>
-      </c>
-      <c r="BL31" t="inlineStr">
-        <is>
-          <t>data\Multi-Illumination\python_a-1-AI-b-1-AI_m3c2_distances.txt</t>
-        </is>
-      </c>
-      <c r="BM31" t="inlineStr">
         <is>
           <t>data\Multi-Illumination\python_a-1-AI-b-1-AI_m3c2_params.txt</t>
         </is>

</xml_diff>